<commit_message>
add method windows event in validation.py
</commit_message>
<xml_diff>
--- a/backend/DSEC/startScan/Compromise_Assesment/Windows/Command_Data/command.xlsx
+++ b/backend/DSEC/startScan/Compromise_Assesment/Windows/Command_Data/command.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DES\DSEC360-\backend\DSEC\startScan\Compromise_Assesment\Windows\Command_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9769EDBE-AEC2-49E8-9311-146380F3EAFC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C6260EC-4659-441E-970B-5D6163B57435}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -569,146 +569,6 @@
   </si>
   <si>
     <t>Configuration Files</t>
-  </si>
-  <si>
-    <t># --- Combined Windows Event Checks ---
-$windowsResults = [ordered]@{}
-# 1. User_Account_Creations
-$StartTime = (Get-Date).AddDays(-7)
-$userEvents = Get-WinEvent -FilterHashtable @{
-    LogName = 'Security';
-    Id = 4720;
-    StartTime = $StartTime
-} | ForEach-Object {
-    $msg = $_.Message
-    $created = if ($msg -match "New Account:\r?\n\s*Security ID:\s*.+?\r?\n\s*Account Name:\s*([^\r\n]+)") {
-        $matches[1].Trim()
-    } else { "N/A" }
-    $creator = if ($msg -match "Subject:\r?\n\s*Security ID:.*\r?\n\s*Account Name:\s*([^\r\n]+)") {
-        $matches[1].Trim()
-    } else { "N/A" }
-    [PSCustomObject]@{
-        Time           = $_.TimeCreated
-        EventID        = $_.Id
-        CreatedAccount = $created
-        CreatorAccount = $creator
-    }
-}
-$windowsResults["User_Account_Creations"] = $userEvents
-# 2. File_Creation_Deletion_Events
-$fileEvents = Get-WinEvent -FilterHashtable @{
-    LogName = 'Security';
-    Id = 4663;
-    StartTime = $StartTime
-} | Where-Object { $_.Message -match 'Accesses:\s+.*(WriteData|Delete)' } |
-ForEach-Object {
-    $object = if ($_.Message -match "Object Name:\s+(.+?)\r") { $matches[1] } else { "N/A" }
-    $access = if ($_.Message -match "Accesses:\s+(.+?)\r") { $matches[1] } else { "N/A" }
-    [PSCustomObject]@{
-        Time    = $_.TimeCreated
-        EventID = $_.Id
-        Object  = $object
-        Access  = $access
-    }
-}
-$windowsResults["File_Creation_Deletion_Events"] = $fileEvents
-# 3. BAT_File_Creation
-$batEvents = Get-WinEvent -FilterHashtable @{
-    LogName = 'Security';
-    Id = 4663;
-    StartTime = $StartTime
-} | Where-Object { $_.Message -match '\.bat' -and $_.Message -match 'WriteData' } |
-ForEach-Object {
-    $object = if ($_.Message -match "Object Name:\s+(.+?\.bat.*?)\r") { $matches[1] } else { "N/A" }
-    $access = if ($_.Message -match "Accesses:\s+(.+?)\r") { $matches[1] } else { "N/A" }
-    [PSCustomObject]@{
-        Time    = $_.TimeCreated
-        EventID = $_.Id
-        Object  = $object
-        Access  = $access
-    }
-}
-$windowsResults["BAT_File_Creation"] = $batEvents
-# 4. Failed_Logon_Attempts
-$logonFailEvents = Get-WinEvent -FilterHashtable @{
-    LogName = 'Security';
-    Id = 4625;
-    StartTime = $StartTime
-} | ForEach-Object {
-    $msg = $_.Message
-    $accountName = if ($msg -match "Account Name:\s+([^\r\n]+)") { $matches[1].Trim() } else { "N/A" }
-    $ipAddress   = if ($msg -match "Source Network Address:\s+([^\r\n]+)") { $matches[1].Trim() } else { "N/A" }
-    $logonType   = if ($msg -match "Logon Type:\s+(\d+)") { $matches[1] } else { "N/A" }
-    $failure     = if ($msg -match "Failure Reason:\s+([^\r\n]+)") { $matches[1].Trim() } else { "N/A" }
-    [PSCustomObject]@{
-        Time          = $_.TimeCreated
-        EventID       = $_.Id
-        Account       = $accountName
-        IPAddress     = $ipAddress
-        LogonType     = $logonType
-        FailureReason = $failure
-    }
-}
-$windowsResults["Failed_Logon_Attempts"] = $logonFailEvents
-# 5. After_Hours_Logons
-$today = [datetime]::Today
-$afterHours = $today.AddHours(18)  # 6 PM
-$afterHourEvents = Get-WinEvent -FilterHashtable @{
-    LogName = 'Security'
-    ID = 4624
-    StartTime = $today
-} | ForEach-Object {
-    $event = [xml]$_.ToXml()
-    $logonTime = $_.TimeCreated
-    $user = $event.Event.EventData.Data | Where-Object { $_.Name -eq "TargetUserName" }
-    if ($logonTime -gt $afterHours -and $user.'#text' -ne 'ANONYMOUS LOGON') {
-        [PSCustomObject]@{
-            TimeCreated = $logonTime
-            UserName    = $user.'#text'
-        }
-    }
-}
-$windowsResults["After_Hours_Logons"] = $afterHourEvents
-# 6. Suspicious_Open_Ports
-$startHour = 9
-$endHour = 18
-$currentHour = (Get-Date).Hour
-$ports = @{
-    "RDP" = 3389
-    "SSH" = 22
-    "FTP" = 21
-}
-function Test-Port {
-    param ([int]$port)
-    try {
-        $tcpClient = New-Object System.Net.Sockets.TcpClient
-        $asyncResult = $tcpClient.BeginConnect("localhost", $port, $null, $null)
-        $wait = $asyncResult.AsyncWaitHandle.WaitOne(2000, $false)
-        if ($wait -and $tcpClient.Connected) {
-            $tcpClient.Close()
-            return $true
-        }
-    } catch {
-        return $false
-    }
-    return $false
-}
-$openPorts = @()
-if ($currentHour -lt $startHour -or $currentHour -ge $endHour) {
-    foreach ($service in $ports.Keys) {
-        $port = $ports[$service]
-        if (Test-Port -port $port) {
-            $openPorts += [PSCustomObject]@{
-                Service = $service
-                Port    = $port
-                Status  = "OPEN"
-            }
-        }
-    }
-}
-$windowsResults["Suspicious_Open_Ports"] = $openPorts
-# Return all grouped results
-$windowsResults</t>
   </si>
   <si>
     <t>PowerShell History</t>
@@ -812,6 +672,151 @@
 }
 # Return array; Run_Check wrapper stores it in $results["Inetpub_Config_Files_Info"]
 $configFiles</t>
+  </si>
+  <si>
+    <t># --- Combined Windows Event Checks ---
+$windowsResults = [ordered]@{}
+# 1. User_Account_Creations
+$StartTime = (Get-Date).AddDays(-7)
+$userEvents = Get-WinEvent -FilterHashtable @{
+    LogName = 'Security';
+    Id = 4720;
+    StartTime = $StartTime
+} | ForEach-Object {
+    $msg = $_.Message
+    $created = if ($msg -match "New Account:\r?\n\s*Security ID:\s*.+?\r?\n\s*Account Name:\s*([^\r\n]+)") {
+        $matches[1].Trim()
+    } else { "N/A" }
+    $creator = if ($msg -match "Subject:\r?\n\s*Security ID:.*\r?\n\s*Account Name:\s*([^\r\n]+)") {
+        $matches[1].Trim()
+    } else { "N/A" }
+    [PSCustomObject]@{
+        Time           = $_.TimeCreated
+        EventID        = $_.Id
+        CreatedAccount = $created
+        CreatorAccount = $creator
+    }
+}
+$windowsResults["User_Account_Creations"] = $userEvents
+# 2. File_Creation_Deletion_Events
+$fileEvents = Get-WinEvent -FilterHashtable @{
+    LogName = 'Security';
+    Id = 4663;
+    StartTime = $StartTime
+} | Where-Object { $_.Message -match 'Accesses:\s+.*(WriteData|Delete)' } |
+ForEach-Object {
+    $object = if ($_.Message -match "Object Name:\s+(.+?)\r") { $matches[1] } else { "N/A" }
+    $access = if ($_.Message -match "Accesses:\s+(.+?)\r") { $matches[1] } else { "N/A" }
+    [PSCustomObject]@{
+        Time    = $_.TimeCreated
+        EventID = $_.Id
+        Object  = $object
+        Access  = $access
+    }
+}
+$windowsResults["File_Creation_Deletion_Events"] = $fileEvents
+# 3. BAT_File_Creation
+$batEvents = Get-WinEvent -FilterHashtable @{
+    LogName = 'Security';
+    Id = 4663;
+    StartTime = $StartTime
+} | Where-Object { $_.Message -match '\.bat' -and $_.Message -match 'WriteData' } |
+ForEach-Object {
+    $object = if ($_.Message -match "Object Name:\s+(.+?\.bat.*?)\r") { $matches[1] } else { "N/A" }
+    $access = if ($_.Message -match "Accesses:\s+(.+?)\r") { $matches[1] } else { "N/A" }
+    [PSCustomObject]@{
+        Time    = $_.TimeCreated
+        EventID = $_.Id
+        Object  = $object
+        Access  = $access
+    }
+}
+$windowsResults["BAT_File_Creation"] = $batEvents
+# 4. Failed_Logon_Attempts
+try {
+    $rawLogonFailEvents = Get-WinEvent -FilterHashtable @{
+        LogName = 'Security';
+        Id = 4625;
+        StartTime = $StartTime
+    } -ErrorAction Stop
+} catch {
+    $rawLogonFailEvents = @()  # Return empty array if no events or error
+}
+$logonFailEvents = $rawLogonFailEvents | ForEach-Object {
+    $msg = $_.Message
+    $accountName = if ($msg -match "Account Name:\s+([^\r\n]+)") { $matches[1].Trim() } else { "N/A" }
+    $ipAddress   = if ($msg -match "Source Network Address:\s+([^\r\n]+)") { $matches[1].Trim() } else { "N/A" }
+    $logonType   = if ($msg -match "Logon Type:\s+(\d+)") { $matches[1] } else { "N/A" }
+    $failure     = if ($msg -match "Failure Reason:\s+([^\r\n]+)") { $matches[1].Trim() } else { "N/A" }
+    [PSCustomObject]@{
+        Time          = $_.TimeCreated
+        EventID       = $_.Id
+        Account       = $accountName
+        IPAddress     = $ipAddress
+        LogonType     = $logonType
+        FailureReason = $failure
+    }
+}
+$windowsResults["Failed_Logon_Attempts"] = $logonFailEvents
+# 5. After_Hours_Logons
+$today = [datetime]::Today
+$afterHours = $today.AddHours(18)  # 6 PM
+$afterHourEvents = Get-WinEvent -FilterHashtable @{
+    LogName = 'Security'
+    ID = 4624
+    StartTime = $today
+} | ForEach-Object {
+    $event = [xml]$_.ToXml()
+    $logonTime = $_.TimeCreated
+    $user = $event.Event.EventData.Data | Where-Object { $_.Name -eq "TargetUserName" }
+    if ($logonTime -gt $afterHours -and $user.'#text' -ne 'ANONYMOUS LOGON') {
+        [PSCustomObject]@{
+            TimeCreated = $logonTime
+            UserName    = $user.'#text'
+        }
+    }
+}
+$windowsResults["After_Hours_Logons"] = $afterHourEvents
+# 6. Suspicious_Open_Ports
+$startHour = 9
+$endHour = 18
+$currentHour = (Get-Date).Hour
+$ports = @{
+    "RDP" = 3389
+    "SSH" = 22
+    "FTP" = 21
+}
+function Test-Port {
+    param ([int]$port)
+    try {
+        $tcpClient = New-Object System.Net.Sockets.TcpClient
+        $asyncResult = $tcpClient.BeginConnect("localhost", $port, $null, $null)
+        $wait = $asyncResult.AsyncWaitHandle.WaitOne(2000, $false)
+        if ($wait -and $tcpClient.Connected) {
+            $tcpClient.Close()
+            return $true
+        }
+    } catch {
+        return $false
+    }
+    return $false
+}
+$openPorts = @()
+if ($currentHour -lt $startHour -or $currentHour -ge $endHour) {
+    foreach ($service in $ports.Keys) {
+        $port = $ports[$service]
+        if (Test-Port -port $port) {
+            $openPorts += [PSCustomObject]@{
+                Service = $service
+                Port    = $port
+                Status  = "OPEN"
+            }
+        }
+    }
+}
+$windowsResults["Suspicious_Open_Ports"] = $openPorts
+# Return all grouped results
+$windowsResults</t>
   </si>
 </sst>
 </file>
@@ -1412,8 +1417,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="72" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="72" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4"/>
@@ -1517,7 +1522,7 @@
         <v>17</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="409.6">
@@ -1550,7 +1555,7 @@
         <v>22</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="409.6">
@@ -1558,10 +1563,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>24</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add Compromise_Assessment.xlsx, add schedule task method in validate.py
</commit_message>
<xml_diff>
--- a/backend/DSEC/startScan/Compromise_Assesment/Windows/Command_Data/command.xlsx
+++ b/backend/DSEC/startScan/Compromise_Assesment/Windows/Command_Data/command.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DES\DSEC360-\backend\DSEC\startScan\Compromise_Assesment\Windows\Command_Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60680A21-7C6C-444A-9808-21198B007E10}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C17D1228-AE7F-4A30-A911-F92A9134DB3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -491,36 +491,6 @@
   </si>
   <si>
     <t>Schedule Task</t>
-  </si>
-  <si>
-    <t># --- Scheduled_Tasks_Info (EXE-based scheduled tasks, paths, status) ---
-$taskList = @()
-# Retrieve all scheduled tasks
-$tasks = Get-ScheduledTask
-foreach ($task in $tasks) {
-    try {
-        # Get task status info
-        $taskInfo = Get-ScheduledTaskInfo -TaskName $task.TaskName -TaskPath $task.TaskPath
-        # Filter to include only EXE-based actions
-        $actions = $task.Actions | Where-Object { $_.Execute -match "\.exe$" }
-        foreach ($action in $actions) {
-            $taskList += [PSCustomObject]@{
-                TaskName    = $task.TaskName
-                TaskPath    = $task.TaskPath
-                Execute     = $action.Execute
-                Arguments   = $action.Arguments
-                WorkingDir  = $action.WorkingDirectory
-                LastRunTime = $taskInfo.LastRunTime
-                NextRunTime = $taskInfo.NextRunTime
-                Status      = $taskInfo.State
-            }
-        }
-    } catch {
-        Write-Warning "⚠️ Failed to retrieve info for task: $($task.TaskName)"
-    }
-}
-# Return array; Run_Check wrapper stores it in $results["Scheduled_Tasks_Info"]
-$taskList</t>
   </si>
   <si>
     <t># --- Local_User_Privileges_Info (Local users with privileges) ---
@@ -817,6 +787,65 @@
 $windowsResults["Suspicious_Open_Ports"] = $openPorts
 # Return all grouped results
 $windowsResults</t>
+  </si>
+  <si>
+    <t># --- Scheduled_Tasks_Info (EXE-based scheduled tasks, paths, status, permissions, hash) ---
+$taskList = @()
+# Retrieve all scheduled tasks
+$tasks = Get-ScheduledTask
+foreach ($task in $tasks) {
+    try {
+        # Get task status info
+        $taskInfo = Get-ScheduledTaskInfo -TaskName $task.TaskName -TaskPath $task.TaskPath
+        # Filter to include only EXE-based actions
+        $actions = $task.Actions | Where-Object { $_.Execute -match "\.exe$" }
+        foreach ($action in $actions) {
+            $exePath = $action.Execute
+            $resolvedPath = $exePath
+            # Attempt to resolve relative paths (e.g., just "cmd.exe" to full path)
+            if (-not (Test-Path $resolvedPath)) {
+                $resolvedPath = (Get-Command $exePath -ErrorAction SilentlyContinue)?.Source
+            }
+            # Initialize default values
+            $fileHash = "N/A"
+            $permissions = "N/A"
+            # Get SHA256 hash
+            if ($resolvedPath -and (Test-Path $resolvedPath)) {
+                try {
+                    $fileHash = (Get-FileHash -Path $resolvedPath -Algorithm SHA256).Hash
+                } catch {
+                    $fileHash = "Hash Error"
+                }
+                # Get permissions
+                try {
+                    $acl = Get-Acl -Path $resolvedPath
+                    $permissions = ($acl.Access | ForEach-Object {
+                        "$($_.IdentityReference):$($_.FileSystemRights)"
+                    }) -join "; "
+                } catch {
+                    $permissions = "Permission Error"
+                }
+            }
+            # Add to results
+            $taskList += [PSCustomObject]@{
+                TaskName    = $task.TaskName
+                TaskPath    = $task.TaskPath
+                Execute     = $exePath
+                Arguments   = $action.Arguments
+                WorkingDir  = $action.WorkingDirectory
+                LastRunTime = $taskInfo.LastRunTime
+                NextRunTime = $taskInfo.NextRunTime
+                Status      = $taskInfo.State
+                Hash        = $fileHash
+                Permissions = $permissions
+            }
+        }
+    } catch {
+        Write-Warning "⚠️ Failed to retrieve info for task: $($task.TaskName)"
+    }
+}
+# Return array; Run_Check wrapper stores it in $results["Scheduled_Tasks_Info"]
+$taskList</t>
   </si>
 </sst>
 </file>
@@ -1522,7 +1551,7 @@
         <v>17</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="409.6">
@@ -1533,7 +1562,7 @@
         <v>18</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="409.6">
@@ -1541,10 +1570,10 @@
         <v>10</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="409.6">
@@ -1552,10 +1581,10 @@
         <v>11</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="409.6">
@@ -1563,10 +1592,10 @@
         <v>12</v>
       </c>
       <c r="B14" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>